<commit_message>
November commit from Leon
</commit_message>
<xml_diff>
--- a/Leon_Contribution_November.xlsx
+++ b/Leon_Contribution_November.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Github-Codes\ULTERA-contribute-Leon\OneDrive_1_2024-11-18\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Github-Codes\ULTERA-contribute-Leon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12192433-25C6-4788-822A-E7B2914E13FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D49DC84-220B-49D2-812E-D7438DCF38E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8743" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="166">
   <si>
     <t>Name:</t>
   </si>
@@ -696,10 +696,6 @@
   </si>
   <si>
     <t>compressive yield strength</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Specify the intermetallic phase</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
@@ -1480,33 +1476,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1556,6 +1525,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1842,7 +1838,7 @@
   <dimension ref="A1:T430"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A86" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F101" sqref="F101"/>
+      <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.45"/>
@@ -1878,19 +1874,19 @@
       <c r="B2" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="60"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="51"/>
       <c r="O2" s="24"/>
     </row>
     <row r="3" spans="1:20" ht="22" customHeight="1" thickBot="1">
@@ -1900,17 +1896,17 @@
       <c r="B3" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="65"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="62"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="53"/>
       <c r="O3" s="24"/>
     </row>
     <row r="4" spans="1:20" ht="22.5" customHeight="1">
@@ -1928,43 +1924,43 @@
       <c r="B5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="75" t="s">
+      <c r="C5" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="56" t="s">
+      <c r="D5" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="56" t="s">
+      <c r="E5" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="56" t="s">
+      <c r="F5" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="56" t="s">
+      <c r="G5" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="57" t="s">
+      <c r="H5" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="56" t="s">
+      <c r="I5" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="56" t="s">
+      <c r="J5" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="56" t="s">
+      <c r="K5" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="L5" s="56" t="s">
+      <c r="L5" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="56" t="s">
+      <c r="M5" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="N5" s="56" t="s">
+      <c r="N5" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="O5" s="50" t="s">
+      <c r="O5" s="68" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1975,19 +1971,19 @@
       <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="56"/>
-      <c r="N6" s="56"/>
-      <c r="O6" s="51"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="75"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="67"/>
+      <c r="N6" s="67"/>
+      <c r="O6" s="69"/>
     </row>
     <row r="7" spans="1:20" ht="17.149999999999999" thickBot="1">
       <c r="A7" s="3" t="s">
@@ -2032,7 +2028,7 @@
       <c r="N7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="52"/>
+      <c r="O7" s="70"/>
       <c r="P7" s="30" t="s">
         <v>40</v>
       </c>
@@ -2045,35 +2041,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="70" t="s">
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="71"/>
-      <c r="H8" s="71"/>
-      <c r="I8" s="71"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="73" t="s">
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="74"/>
+      <c r="N8" s="65"/>
       <c r="O8" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="P8" s="53" t="s">
+      <c r="P8" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="Q8" s="54"/>
-      <c r="R8" s="54"/>
-      <c r="S8" s="54"/>
-      <c r="T8" s="55"/>
+      <c r="Q8" s="72"/>
+      <c r="R8" s="72"/>
+      <c r="S8" s="72"/>
+      <c r="T8" s="73"/>
     </row>
     <row r="9" spans="1:20" ht="22" customHeight="1" thickBot="1">
       <c r="A9" s="2" t="s">
@@ -3130,7 +3126,7 @@
         <v>102</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D37" s="32" t="s">
         <v>75</v>
@@ -3166,7 +3162,7 @@
         <v>104</v>
       </c>
       <c r="C38" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D38" s="32" t="s">
         <v>75</v>
@@ -3202,7 +3198,7 @@
         <v>105</v>
       </c>
       <c r="C39" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D39" s="32" t="s">
         <v>75</v>
@@ -3238,7 +3234,7 @@
         <v>106</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D40" s="32" t="s">
         <v>75</v>
@@ -3274,7 +3270,7 @@
         <v>107</v>
       </c>
       <c r="C41" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D41" s="32" t="s">
         <v>75</v>
@@ -3310,7 +3306,7 @@
         <v>108</v>
       </c>
       <c r="C42" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D42" s="32" t="s">
         <v>75</v>
@@ -3346,7 +3342,7 @@
         <v>109</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D43" s="32" t="s">
         <v>75</v>
@@ -3382,7 +3378,7 @@
         <v>110</v>
       </c>
       <c r="C44" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D44" s="32" t="s">
         <v>75</v>
@@ -3418,7 +3414,7 @@
         <v>111</v>
       </c>
       <c r="C45" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D45" s="32" t="s">
         <v>75</v>
@@ -3454,7 +3450,7 @@
         <v>112</v>
       </c>
       <c r="C46" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D46" s="32" t="s">
         <v>75</v>
@@ -3490,7 +3486,7 @@
         <v>113</v>
       </c>
       <c r="C47" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D47" s="32" t="s">
         <v>75</v>
@@ -3526,7 +3522,7 @@
         <v>114</v>
       </c>
       <c r="C48" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D48" s="32" t="s">
         <v>75</v>
@@ -3562,7 +3558,7 @@
         <v>115</v>
       </c>
       <c r="C49" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D49" s="32" t="s">
         <v>75</v>
@@ -3598,7 +3594,7 @@
         <v>116</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D50" s="32" t="s">
         <v>75</v>
@@ -3634,7 +3630,7 @@
         <v>117</v>
       </c>
       <c r="C51" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D51" s="32" t="s">
         <v>75</v>
@@ -3670,7 +3666,7 @@
         <v>118</v>
       </c>
       <c r="C52" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D52" s="32" t="s">
         <v>75</v>
@@ -3708,7 +3704,7 @@
         <v>102</v>
       </c>
       <c r="C53" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D53" s="32" t="s">
         <v>75</v>
@@ -3744,7 +3740,7 @@
         <v>104</v>
       </c>
       <c r="C54" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D54" s="32" t="s">
         <v>75</v>
@@ -3780,7 +3776,7 @@
         <v>105</v>
       </c>
       <c r="C55" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D55" s="32" t="s">
         <v>75</v>
@@ -3816,7 +3812,7 @@
         <v>106</v>
       </c>
       <c r="C56" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D56" s="32" t="s">
         <v>75</v>
@@ -3852,7 +3848,7 @@
         <v>107</v>
       </c>
       <c r="C57" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D57" s="32" t="s">
         <v>75</v>
@@ -3888,7 +3884,7 @@
         <v>108</v>
       </c>
       <c r="C58" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D58" s="32" t="s">
         <v>75</v>
@@ -3924,7 +3920,7 @@
         <v>109</v>
       </c>
       <c r="C59" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D59" s="32" t="s">
         <v>75</v>
@@ -3960,7 +3956,7 @@
         <v>110</v>
       </c>
       <c r="C60" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D60" s="32" t="s">
         <v>75</v>
@@ -3996,7 +3992,7 @@
         <v>111</v>
       </c>
       <c r="C61" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D61" s="32" t="s">
         <v>75</v>
@@ -4032,7 +4028,7 @@
         <v>112</v>
       </c>
       <c r="C62" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D62" s="32" t="s">
         <v>75</v>
@@ -4068,7 +4064,7 @@
         <v>113</v>
       </c>
       <c r="C63" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D63" s="32" t="s">
         <v>75</v>
@@ -4104,7 +4100,7 @@
         <v>114</v>
       </c>
       <c r="C64" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D64" s="32" t="s">
         <v>75</v>
@@ -4750,7 +4746,7 @@
         <v>149</v>
       </c>
       <c r="C82" s="32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D82" s="32" t="s">
         <v>75</v>
@@ -4779,7 +4775,7 @@
         <v>154</v>
       </c>
       <c r="N82" s="44" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="83" spans="1:14" ht="16.3">
@@ -4788,7 +4784,7 @@
         <v>150</v>
       </c>
       <c r="C83" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D83" s="32" t="s">
         <v>75</v>
@@ -4817,7 +4813,7 @@
         <v>154</v>
       </c>
       <c r="N83" s="44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="84" spans="1:14" ht="16.3">
@@ -4826,7 +4822,7 @@
         <v>151</v>
       </c>
       <c r="C84" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D84" s="32" t="s">
         <v>75</v>
@@ -4855,7 +4851,7 @@
         <v>154</v>
       </c>
       <c r="N84" s="44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="85" spans="1:14" ht="16.3">
@@ -4864,7 +4860,7 @@
         <v>152</v>
       </c>
       <c r="C85" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D85" s="32" t="s">
         <v>75</v>
@@ -4893,7 +4889,7 @@
         <v>154</v>
       </c>
       <c r="N85" s="44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="86" spans="1:14" ht="16.3">
@@ -4902,7 +4898,7 @@
         <v>153</v>
       </c>
       <c r="C86" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D86" s="32" t="s">
         <v>75</v>
@@ -4931,7 +4927,7 @@
         <v>154</v>
       </c>
       <c r="N86" s="44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="87" spans="1:14" ht="16.3">
@@ -4940,7 +4936,7 @@
         <v>149</v>
       </c>
       <c r="C87" s="32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D87" s="32" t="s">
         <v>75</v>
@@ -4964,10 +4960,10 @@
         <v>79</v>
       </c>
       <c r="M87" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="N87" s="44" t="s">
         <v>159</v>
-      </c>
-      <c r="N87" s="44" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="88" spans="1:14" ht="16.3">
@@ -4976,7 +4972,7 @@
         <v>150</v>
       </c>
       <c r="C88" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D88" s="32" t="s">
         <v>75</v>
@@ -5000,10 +4996,10 @@
         <v>79</v>
       </c>
       <c r="M88" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="N88" s="44" t="s">
         <v>159</v>
-      </c>
-      <c r="N88" s="44" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="89" spans="1:14" ht="16.3">
@@ -5012,7 +5008,7 @@
         <v>151</v>
       </c>
       <c r="C89" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D89" s="32" t="s">
         <v>75</v>
@@ -5036,10 +5032,10 @@
         <v>79</v>
       </c>
       <c r="M89" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N89" s="44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="90" spans="1:14" ht="16.3">
@@ -5048,7 +5044,7 @@
         <v>152</v>
       </c>
       <c r="C90" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D90" s="32" t="s">
         <v>75</v>
@@ -5072,10 +5068,10 @@
         <v>79</v>
       </c>
       <c r="M90" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N90" s="44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="91" spans="1:14" ht="16.3">
@@ -5084,7 +5080,7 @@
         <v>153</v>
       </c>
       <c r="C91" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D91" s="32" t="s">
         <v>75</v>
@@ -5108,10 +5104,10 @@
         <v>79</v>
       </c>
       <c r="M91" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N91" s="44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="92" spans="1:14" ht="16.3">
@@ -5120,7 +5116,7 @@
         <v>149</v>
       </c>
       <c r="C92" s="32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D92" s="32" t="s">
         <v>75</v>
@@ -5144,10 +5140,10 @@
         <v>79</v>
       </c>
       <c r="M92" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N92" s="44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="93" spans="1:14" ht="16.3">
@@ -5156,7 +5152,7 @@
         <v>150</v>
       </c>
       <c r="C93" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D93" s="32" t="s">
         <v>75</v>
@@ -5180,10 +5176,10 @@
         <v>79</v>
       </c>
       <c r="M93" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N93" s="44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="94" spans="1:14" ht="16.3">
@@ -5192,7 +5188,7 @@
         <v>151</v>
       </c>
       <c r="C94" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D94" s="32" t="s">
         <v>75</v>
@@ -5216,10 +5212,10 @@
         <v>79</v>
       </c>
       <c r="M94" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N94" s="44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="95" spans="1:14" ht="16.3">
@@ -5228,7 +5224,7 @@
         <v>152</v>
       </c>
       <c r="C95" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D95" s="32" t="s">
         <v>75</v>
@@ -5252,10 +5248,10 @@
         <v>79</v>
       </c>
       <c r="M95" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N95" s="44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="96" spans="1:14" ht="16.3">
@@ -5264,7 +5260,7 @@
         <v>153</v>
       </c>
       <c r="C96" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D96" s="32" t="s">
         <v>75</v>
@@ -5288,10 +5284,10 @@
         <v>79</v>
       </c>
       <c r="M96" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N96" s="44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="97" spans="1:14" ht="16.3">
@@ -5300,7 +5296,7 @@
         <v>151</v>
       </c>
       <c r="C97" s="32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D97" s="32" t="s">
         <v>75</v>
@@ -5324,10 +5320,10 @@
         <v>73</v>
       </c>
       <c r="M97" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N97" s="44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="98" spans="1:14" ht="16.3">
@@ -5336,7 +5332,7 @@
         <v>152</v>
       </c>
       <c r="C98" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D98" s="32" t="s">
         <v>75</v>
@@ -5360,10 +5356,10 @@
         <v>73</v>
       </c>
       <c r="M98" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N98" s="44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="99" spans="1:14" ht="16.3">
@@ -5372,7 +5368,7 @@
         <v>153</v>
       </c>
       <c r="C99" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D99" s="32" t="s">
         <v>75</v>
@@ -5396,10 +5392,10 @@
         <v>73</v>
       </c>
       <c r="M99" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N99" s="44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="100" spans="1:14" ht="16.3">
@@ -5419,9 +5415,7 @@
     </row>
     <row r="101" spans="1:14" ht="16.3">
       <c r="A101" s="35"/>
-      <c r="B101" s="19" t="s">
-        <v>157</v>
-      </c>
+      <c r="B101" s="19"/>
       <c r="C101" s="32"/>
       <c r="D101" s="32"/>
       <c r="E101" s="19"/>
@@ -10148,6 +10142,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="H5:H6"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="B8:E8"/>
@@ -10162,11 +10161,6 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="L5:L6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Correction of property name
</commit_message>
<xml_diff>
--- a/Leon_Contribution_November.xlsx
+++ b/Leon_Contribution_November.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Github-Codes\ULTERA-contribute-Leon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB60D3B6-4921-432D-98DC-B2BE49FB25FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD98A3DD-3D93-4058-93B8-AF9571E907F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8743" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="171">
   <si>
     <t>Name:</t>
   </si>
@@ -776,6 +776,10 @@
       </rPr>
       <t xml:space="preserve"> Y</t>
     </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.1016/j.matchar.2024.114393</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
@@ -1571,6 +1575,34 @@
     <xf numFmtId="49" fontId="15" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1622,34 +1654,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1934,7 +1938,7 @@
   <dimension ref="A1:T430"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.45"/>
@@ -1970,19 +1974,19 @@
       <c r="B2" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="66" t="s">
+      <c r="D2" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="67"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="63"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="73"/>
       <c r="O2" s="24"/>
     </row>
     <row r="3" spans="1:20" ht="22" customHeight="1" thickBot="1">
@@ -1992,17 +1996,17 @@
       <c r="B3" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="68"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="64"/>
-      <c r="N3" s="65"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="75"/>
       <c r="O3" s="24"/>
     </row>
     <row r="4" spans="1:20" ht="22.5" customHeight="1">
@@ -2020,43 +2024,43 @@
       <c r="B5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="78" t="s">
+      <c r="C5" s="88" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="79" t="s">
+      <c r="D5" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="79" t="s">
+      <c r="E5" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="79" t="s">
+      <c r="F5" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="79" t="s">
+      <c r="G5" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="86" t="s">
+      <c r="H5" s="70" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="79" t="s">
+      <c r="I5" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="79" t="s">
+      <c r="J5" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="79" t="s">
+      <c r="K5" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="L5" s="79" t="s">
+      <c r="L5" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="79" t="s">
+      <c r="M5" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="N5" s="79" t="s">
+      <c r="N5" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="O5" s="80" t="s">
+      <c r="O5" s="63" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2067,19 +2071,19 @@
       <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="79"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="79"/>
-      <c r="J6" s="79"/>
-      <c r="K6" s="79"/>
-      <c r="L6" s="79"/>
-      <c r="M6" s="79"/>
-      <c r="N6" s="79"/>
-      <c r="O6" s="81"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="69"/>
+      <c r="L6" s="69"/>
+      <c r="M6" s="69"/>
+      <c r="N6" s="69"/>
+      <c r="O6" s="64"/>
     </row>
     <row r="7" spans="1:20" ht="17.149999999999999" thickBot="1">
       <c r="A7" s="3" t="s">
@@ -2124,7 +2128,7 @@
       <c r="N7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="82"/>
+      <c r="O7" s="65"/>
       <c r="P7" s="30" t="s">
         <v>40</v>
       </c>
@@ -2137,35 +2141,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="70" t="s">
+      <c r="B8" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="73" t="s">
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="74"/>
-      <c r="H8" s="74"/>
-      <c r="I8" s="74"/>
-      <c r="J8" s="75"/>
-      <c r="K8" s="75"/>
-      <c r="L8" s="75"/>
-      <c r="M8" s="76" t="s">
+      <c r="G8" s="84"/>
+      <c r="H8" s="84"/>
+      <c r="I8" s="84"/>
+      <c r="J8" s="85"/>
+      <c r="K8" s="85"/>
+      <c r="L8" s="85"/>
+      <c r="M8" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="77"/>
+      <c r="N8" s="87"/>
       <c r="O8" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="P8" s="83" t="s">
+      <c r="P8" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="Q8" s="84"/>
-      <c r="R8" s="84"/>
-      <c r="S8" s="84"/>
-      <c r="T8" s="85"/>
+      <c r="Q8" s="67"/>
+      <c r="R8" s="67"/>
+      <c r="S8" s="67"/>
+      <c r="T8" s="68"/>
     </row>
     <row r="9" spans="1:20" ht="22" customHeight="1" thickBot="1">
       <c r="A9" s="2" t="s">
@@ -2265,7 +2269,7 @@
         <v>70</v>
       </c>
       <c r="O10" s="19"/>
-      <c r="P10" s="88"/>
+      <c r="P10" s="62"/>
     </row>
     <row r="11" spans="1:20" ht="16.3">
       <c r="A11" s="36"/>
@@ -2892,7 +2896,7 @@
       </c>
       <c r="E26" s="19"/>
       <c r="F26" s="32" t="s">
-        <v>133</v>
+        <v>71</v>
       </c>
       <c r="G26" s="40" t="s">
         <v>78</v>
@@ -3091,7 +3095,7 @@
         <v>89</v>
       </c>
       <c r="E31" s="19"/>
-      <c r="F31" s="47" t="s">
+      <c r="F31" s="32" t="s">
         <v>71</v>
       </c>
       <c r="G31" s="40" t="s">
@@ -3112,7 +3116,7 @@
         <v>98</v>
       </c>
       <c r="N31" s="44" t="s">
-        <v>101</v>
+        <v>170</v>
       </c>
       <c r="P31" t="b" cm="1">
         <f t="array" ref="P31">AND(ISNUMBER(SEARCH("Pa",CONCATENATE($A31:$O31))),ISNUMBER(SEARCH("compressive ductility",CONCATENATE($A31:$O31))))</f>
@@ -3291,7 +3295,7 @@
         <v>89</v>
       </c>
       <c r="E36" s="19"/>
-      <c r="F36" s="47" t="s">
+      <c r="F36" s="32" t="s">
         <v>71</v>
       </c>
       <c r="G36" s="40" t="s">
@@ -10595,11 +10599,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="H5:H6"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="B8:E8"/>
@@ -10614,6 +10613,11 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="L5:L6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="A47:O47 Q47:XFD47">

</xml_diff>

<commit_message>
Correction of property names
</commit_message>
<xml_diff>
--- a/Leon_Contribution_November.xlsx
+++ b/Leon_Contribution_November.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Github-Codes\ULTERA-contribute-Leon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD98A3DD-3D93-4058-93B8-AF9571E907F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FCF9B4-ABE6-4130-A7F7-5578F2DF9DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8743" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="172">
   <si>
     <t>Name:</t>
   </si>
@@ -784,6 +784,10 @@
   </si>
   <si>
     <t>10.1016/j.matchar.2024.114393</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ultimate compressive strength</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -1576,33 +1580,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1652,6 +1629,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1938,7 +1942,7 @@
   <dimension ref="A1:T430"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.45"/>
@@ -1974,19 +1978,19 @@
       <c r="B2" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="76" t="s">
+      <c r="D2" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="77"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="73"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="64"/>
       <c r="O2" s="24"/>
     </row>
     <row r="3" spans="1:20" ht="22" customHeight="1" thickBot="1">
@@ -1996,17 +2000,17 @@
       <c r="B3" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="78"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
-      <c r="L3" s="74"/>
-      <c r="M3" s="74"/>
-      <c r="N3" s="75"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+      <c r="N3" s="66"/>
       <c r="O3" s="24"/>
     </row>
     <row r="4" spans="1:20" ht="22.5" customHeight="1">
@@ -2024,43 +2028,43 @@
       <c r="B5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="88" t="s">
+      <c r="C5" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="69" t="s">
+      <c r="D5" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="69" t="s">
+      <c r="E5" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="69" t="s">
+      <c r="F5" s="80" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="69" t="s">
+      <c r="G5" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="70" t="s">
+      <c r="H5" s="87" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="69" t="s">
+      <c r="I5" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="69" t="s">
+      <c r="J5" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="69" t="s">
+      <c r="K5" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="L5" s="69" t="s">
+      <c r="L5" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="69" t="s">
+      <c r="M5" s="80" t="s">
         <v>59</v>
       </c>
-      <c r="N5" s="69" t="s">
+      <c r="N5" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="O5" s="63" t="s">
+      <c r="O5" s="81" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2071,19 +2075,19 @@
       <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="69"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="69"/>
-      <c r="L6" s="69"/>
-      <c r="M6" s="69"/>
-      <c r="N6" s="69"/>
-      <c r="O6" s="64"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="80"/>
+      <c r="M6" s="80"/>
+      <c r="N6" s="80"/>
+      <c r="O6" s="82"/>
     </row>
     <row r="7" spans="1:20" ht="17.149999999999999" thickBot="1">
       <c r="A7" s="3" t="s">
@@ -2128,7 +2132,7 @@
       <c r="N7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="65"/>
+      <c r="O7" s="83"/>
       <c r="P7" s="30" t="s">
         <v>40</v>
       </c>
@@ -2141,35 +2145,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="81"/>
-      <c r="D8" s="81"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="83" t="s">
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="84"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="84"/>
-      <c r="J8" s="85"/>
-      <c r="K8" s="85"/>
-      <c r="L8" s="85"/>
-      <c r="M8" s="86" t="s">
+      <c r="G8" s="75"/>
+      <c r="H8" s="75"/>
+      <c r="I8" s="75"/>
+      <c r="J8" s="76"/>
+      <c r="K8" s="76"/>
+      <c r="L8" s="76"/>
+      <c r="M8" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="87"/>
+      <c r="N8" s="78"/>
       <c r="O8" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="P8" s="66" t="s">
+      <c r="P8" s="84" t="s">
         <v>39</v>
       </c>
-      <c r="Q8" s="67"/>
-      <c r="R8" s="67"/>
-      <c r="S8" s="67"/>
-      <c r="T8" s="68"/>
+      <c r="Q8" s="85"/>
+      <c r="R8" s="85"/>
+      <c r="S8" s="85"/>
+      <c r="T8" s="86"/>
     </row>
     <row r="9" spans="1:20" ht="22" customHeight="1" thickBot="1">
       <c r="A9" s="2" t="s">
@@ -2896,7 +2900,7 @@
       </c>
       <c r="E26" s="19"/>
       <c r="F26" s="32" t="s">
-        <v>71</v>
+        <v>171</v>
       </c>
       <c r="G26" s="40" t="s">
         <v>78</v>
@@ -3096,7 +3100,7 @@
       </c>
       <c r="E31" s="19"/>
       <c r="F31" s="32" t="s">
-        <v>71</v>
+        <v>171</v>
       </c>
       <c r="G31" s="40" t="s">
         <v>78</v>
@@ -3296,7 +3300,7 @@
       </c>
       <c r="E36" s="19"/>
       <c r="F36" s="32" t="s">
-        <v>71</v>
+        <v>171</v>
       </c>
       <c r="G36" s="40" t="s">
         <v>78</v>
@@ -10599,6 +10603,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="H5:H6"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="B8:E8"/>
@@ -10613,11 +10622,6 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="L5:L6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="A47:O47 Q47:XFD47">

</xml_diff>